<commit_message>
1.change symbol setting structure(json file); 2.fixed SymbolData.merge_data to calculate if basis is not in data index; 3.update analyzing for history trend of RB; 4.add data index for 焦炭
</commit_message>
<xml_diff>
--- a/steel/data/up-stream/铁矿石/铁矿石价格.xlsx
+++ b/steel/data/up-stream/铁矿石/铁矿石价格.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Repository\Projects\ffa\data\钢铁产业链\上游数据\铁矿石\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Repository\Projects\ffa\steel\data\up-stream\铁矿石\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55D7199-E2F2-4DC2-AA63-05D2E683D834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C121AD-3648-4FD7-8921-1D21E0253E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="277" windowWidth="38596" windowHeight="20146" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1837" yWindow="2213" windowWidth="28800" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <author>howard</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{7F301E35-A900-4221-BF9C-4B3724AEECBA}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D460C406-EAB3-4A46-87A0-6159979CE164}">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
             <family val="3"/>
             <charset val="134"/>
           </rPr>
-          <t>yVjpCgZpNvMnx10WKQG33+WbK/LBks72hZwANFaVEVeWADzVSfIyXSs+w5Fw75R+44ku45gkXQEu7RiTVhaWte4tbOHkPZpzyHNE8PH+svnXKBVD6AdbGv8xzrnrTnQ/7ns98v8w7HD3yDa5YmlLxhPo9ZygYCJbHtkvsi/WvjGYvk03pxOU6dVakxJwIZKhOEvUu7YXXJ0kLE99Z2Tv+4HvQL4KiiomB5TNAvJO2V8LQJVmUqBPLhZXGHJJcjy2J/XYj7pUlEtENc9aerIucYAbXvRdv5Vk9L0mFXN3+hEQp8Lbj36T6Pe0kMWNg1kqvWdyRQ4cL+l0y842OBjjCpEWgd2oOfPi6R4l2JO5kKyblx0XF3bK4nMrfpBB/LfzXMDVAMnuCDYn1kizjMszzo8fh+dmJb/ZNrTmq1uetqXbWsqC9h0wdu32WVTam0mwOEsG4jalhvPFIC6/TLx8D/FU36S0TWHtvqBnFijm49e7rozelHW5x+LV2phlMV3yBGL69Q3yR7xIId8yM/Xu8eJ5OEPK+DkX8/TZX4/XDlHdnWkPOLkHvnTGyCtg21ekMV42GwY1ak9WL01NzFp+E0RRwS7KXs7u30ZOpBqJ0iU9Jvi1IS6/2GCwXDWMLMKCElCpzg9UiMsfR0yhTIpyKVNDXa3dcGmYmDOYwu5OLAq00WVBUlZ0TC1AW/3gJCM9DFO5G45IwPiYYzWBSNMZaktSqZDAkH86mbg5yEkE6jIN5J3k3EDbM3ZE6rlkByGITx649UBWdbOoj/IZnaINKUJMgzhwKYCrXVLLs1L2Beq906MgNtrYkBlysG5zIjuGMBpGQdQGRE3a5hLe28P6I+Ay6ej+niXn3HgqyCR4kpqgWwmcEgySW1VZWGyKg49t5QhKH9f603aMoTKno9eTWfDT5S1bqoILHNRHjFRnlxnZq+dqeGMGXyvcF/TcC5S8yiRBCHcaz0biUl9n4kB+Qmz8uIGuXPrb7I93CMgfHHj3IdiOBB8QcyOFXRnzaTamLjJRncDRJ81OsHK+NKbPLdmh4+g4UgLPyTy8WmlESFXzFFk5+TKtB9HnP5Js1PgsuGx07Wu/ATzXtJIONDQdGLmLfgiiUVO7BYrCbc/Opj+pbk53+3Fln0yPtZWW0sdXximkFKi88DByI22GpoBw/0zoEvq0gPqeACoFfOmgWgbdhMeeg0mYE+aCD5cwIn03ZOzOWmH0vpW9yYUxUfOt42XzVhjz/Bk8U+g7S8+a5/QL/MLmtwdsm/PeofZACqiX+vDz5u/IJ/ZGj3K4TG0gisYdNEuW5gOw2hv+l+ZjNFM=</t>
+          <t>yVjpCgZpNvMnx10WKQG33zgpka4ckcDNzDFhEQrzY3eHPJy5zv8YWUBOcw4CJZsgEi9gBeYd64E3MZ9NbV3GwSHQmintNPh9sc/2QQcVgi9/dIPenqUcZdZjkHFH13cGemEP//+9J/j3st7Q6PKQ2Do94omQe0MMb3pmUquTtH6+d4uXBzeJdxn85XfG/lgWJbvbcgajvlmONXKiPCfSuZHSzoBsqc/mnrNYUTeUfBgLykTSlfajF0Hb+PSf1bOupw+SBNVaQA/M0snq/TSZT7qnHccWP1L6QANsj5RJ7tSt7GTFjYsQToS0+xBuGOaCqjUCJU/xhS7Z2v/rhieZwri2Gws7Po+O8hrYsU1ZdNhZm/EG94vyi2pel1OUbvV9YwYOGu1+iLNPh2C01uDQ0LF2Xk+Xr+BHzv24AsqLhsrZ3HBejHuNVTsfmUbvln7MbWD7ILsJx60rCYSz6byUeIZ7HdipS771rSWcMPtsjcGful+a9F0oLbU6TQNRMxBvCFr8bbb1qngSK4TDGUYCVn0VuDMRz+DJaIvBwpE7T3uFn/4+AOSTkjXTa6idslqB2nAHxJp/IeKEcuSpvrSNorfpxL66UrSrXAHG/svAqv3ccP4FxQ0vtnCjQhWwdlPtNv4t9ohQy3YDC4eyj3lmHEajXR+ImecqNKnQOLlNsp+kyPJo9BY7CkqkjsmSZIncZaN6XReE34syyYETw/VmdK1Hk54K8oQjcw8PigbOZ/W3zWice9t8WH2wizi5p8Gv2U7aeY+ZwV/5iY9t+MGBB4r5YluuzCx8ULgFGKVLL8Fj2jT0KMpr2k4RWgDNvdTIWesvF7XyufOcB+S2waJIUaCw9+hBeez8Qx0o+w+Hn/MycBgf7qORGS7f25vD+pITpVrbkdMkM10sal7JeZZeYi0GwCDH2xjBmxRzScupTQICm3lF3xDQAM8Oi3AUxaJQUmJ8IGXUeyLdIGpgxWzxbqO6WehWH9Rv7+jH8cabrGVF1a3MVsrPypB1VT5esEEFTHpccvkDiQ25p9/70vffetgU7xiVOuMpCu78fY1Cnqx23bqCFkvgDJF84B4ahML/nh8y5H/NN2fp1qTDYwAsv7254mnJK/80hTDVfy3OYiudhMWtMRvqgDrH42djYTBxSkfxBz2ymdz4tQ3RFxk/2ne0vkEaqKcZv7wYr/Cd9Ct4GEcfE5fwTcpq/BhVifA05GSGPUswVQAtEJk6Y5Wy/JWZUND+03RZfLNSPNfKJjl06TB8JXIlx/csNDbSBUt7nv/pWRyiLWBawAz9QRFMl7ZxlQHTLwdE3RGmoJkfamA=</t>
         </r>
       </text>
     </comment>
@@ -110,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -247,7 +247,7 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -753,11 +753,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F3402"/>
+  <dimension ref="A1:F3412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3348" workbookViewId="0">
-      <selection activeCell="F3402" sqref="F3402"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -63487,8 +63485,204 @@
         <v>850</v>
       </c>
     </row>
-    <row r="3402" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3402" s="2" t="s">
+    <row r="3400" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3400" s="5">
+        <v>45250</v>
+      </c>
+      <c r="B3400" s="6">
+        <v>920</v>
+      </c>
+      <c r="C3400" s="6">
+        <v>880</v>
+      </c>
+      <c r="D3400" s="6">
+        <v>982</v>
+      </c>
+      <c r="E3400" s="6">
+        <v>1092</v>
+      </c>
+      <c r="F3400" s="6">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="3401" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3401" s="5">
+        <v>45251</v>
+      </c>
+      <c r="B3401" s="6">
+        <v>925</v>
+      </c>
+      <c r="C3401" s="6">
+        <v>890</v>
+      </c>
+      <c r="D3401" s="6">
+        <v>1002</v>
+      </c>
+      <c r="E3401" s="6">
+        <v>1100</v>
+      </c>
+      <c r="F3401" s="6">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="3402" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3402" s="5">
+        <v>45252</v>
+      </c>
+      <c r="B3402" s="6">
+        <v>925</v>
+      </c>
+      <c r="C3402" s="6">
+        <v>890</v>
+      </c>
+      <c r="D3402" s="6">
+        <v>1002</v>
+      </c>
+      <c r="E3402" s="6">
+        <v>1102</v>
+      </c>
+      <c r="F3402" s="6">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="3403" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3403" s="5">
+        <v>45253</v>
+      </c>
+      <c r="B3403" s="6">
+        <v>935</v>
+      </c>
+      <c r="C3403" s="6">
+        <v>900</v>
+      </c>
+      <c r="D3403" s="6">
+        <v>1000</v>
+      </c>
+      <c r="E3403" s="6">
+        <v>1094</v>
+      </c>
+      <c r="F3403" s="6">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="3404" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3404" s="5">
+        <v>45254</v>
+      </c>
+      <c r="B3404" s="6">
+        <v>935</v>
+      </c>
+      <c r="C3404" s="6">
+        <v>910</v>
+      </c>
+      <c r="D3404" s="6">
+        <v>995</v>
+      </c>
+      <c r="E3404" s="6">
+        <v>1088</v>
+      </c>
+      <c r="F3404" s="6">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="3405" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3405" s="5">
+        <v>45257</v>
+      </c>
+      <c r="B3405" s="6">
+        <v>935</v>
+      </c>
+      <c r="C3405" s="6">
+        <v>910</v>
+      </c>
+      <c r="D3405" s="6">
+        <v>993</v>
+      </c>
+      <c r="E3405" s="6">
+        <v>1089</v>
+      </c>
+      <c r="F3405" s="6">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="3406" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3406" s="5">
+        <v>45258</v>
+      </c>
+      <c r="B3406" s="6">
+        <v>935</v>
+      </c>
+      <c r="C3406" s="6">
+        <v>910</v>
+      </c>
+      <c r="D3406" s="6">
+        <v>988</v>
+      </c>
+      <c r="E3406" s="6">
+        <v>1083</v>
+      </c>
+      <c r="F3406" s="6">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="3407" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3407" s="5">
+        <v>45259</v>
+      </c>
+      <c r="B3407" s="6">
+        <v>930</v>
+      </c>
+      <c r="C3407" s="6">
+        <v>910</v>
+      </c>
+      <c r="D3407" s="6">
+        <v>980</v>
+      </c>
+      <c r="E3407" s="6">
+        <v>1079</v>
+      </c>
+      <c r="F3407" s="6">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="3408" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3408" s="5">
+        <v>45260</v>
+      </c>
+      <c r="B3408" s="6">
+        <v>930</v>
+      </c>
+      <c r="C3408" s="6">
+        <v>910</v>
+      </c>
+      <c r="D3408" s="6">
+        <v>972</v>
+      </c>
+      <c r="E3408" s="6">
+        <v>1067</v>
+      </c>
+      <c r="F3408" s="6">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="3409" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3409" s="5">
+        <v>45261</v>
+      </c>
+      <c r="B3409" s="6"/>
+      <c r="C3409" s="6"/>
+      <c r="D3409" s="6">
+        <v>985</v>
+      </c>
+      <c r="E3409" s="6">
+        <v>1077</v>
+      </c>
+      <c r="F3409" s="6">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="3412" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3412" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>